<commit_message>
Updated with MTF from UHR (U95). Adjustments to Excel files.
</commit_message>
<xml_diff>
--- a/ExcelTemplates/getSiemensQC_CT_template.xlsx
+++ b/ExcelTemplates/getSiemensQC_CT_template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="165" windowWidth="14115" windowHeight="15840"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -98,7 +98,13 @@
     <t>Lab</t>
   </si>
   <si>
-    <t>PET-CT lab 19</t>
+    <t>MTF50 U95u</t>
+  </si>
+  <si>
+    <t>MTF10 U95u</t>
+  </si>
+  <si>
+    <t>xx</t>
   </si>
 </sst>
 </file>
@@ -186,7 +192,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -313,8 +329,10 @@
             <c:v>Head</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:xVal>
@@ -344,8 +362,10 @@
             <c:v>Body</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -436,11 +456,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="79329152"/>
-        <c:axId val="98504704"/>
+        <c:axId val="42443904"/>
+        <c:axId val="42445440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="79329152"/>
+        <c:axId val="42443904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -460,13 +480,13 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98504704"/>
+        <c:crossAx val="42445440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="30"/>
+        <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98504704"/>
+        <c:axId val="42445440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -496,7 +516,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79329152"/>
+        <c:crossAx val="42443904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
@@ -505,6 +525,291 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="nb-NO"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>MTF</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 10% sharp UHR</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11404906290658777"/>
+          <c:y val="0.14030471800781"/>
+          <c:w val="0.63436816538584473"/>
+          <c:h val="0.70648357979642784"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Head</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Table!$A$12:$A$1000</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="989"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Table!$X$12:$X$1000</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="989"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>tol min head</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Table!$A$12,Table!$A$10)</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Table!$X$6,Table!$X$6)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>20.47</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.47</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>tol max head</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Table!$A$12,Table!$A$10)</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Table!$X$7,Table!$X$7)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>25.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="216067072"/>
+        <c:axId val="216068864"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="216067072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="[$-414]mmm\.\ yy;@" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="2700000"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="216068864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="90"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="216068864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="26"/>
+          <c:min val="19"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>MTF</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> 10% (lp/mm)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="216067072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.77338321560576795"/>
+          <c:y val="8.0795083541386592E-2"/>
+          <c:w val="0.20707878067557164"/>
+          <c:h val="0.58806222392932594"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -575,8 +880,10 @@
             <c:v>Head</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:xVal>
@@ -606,8 +913,10 @@
             <c:v>Body</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -836,11 +1145,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="54511488"/>
-        <c:axId val="54513024"/>
+        <c:axId val="55020544"/>
+        <c:axId val="213975808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="54511488"/>
+        <c:axId val="55020544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -860,13 +1169,13 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54513024"/>
+        <c:crossAx val="213975808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="30"/>
+        <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="54513024"/>
+        <c:axId val="213975808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -903,7 +1212,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54511488"/>
+        <c:crossAx val="55020544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -991,8 +1300,10 @@
             <c:v>Head min</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:xVal>
@@ -1022,8 +1333,10 @@
             <c:v>Head max</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -1065,8 +1378,10 @@
             <c:v>Body min</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -1110,8 +1425,10 @@
             <c:v>Body max</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -1338,11 +1655,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="77587968"/>
-        <c:axId val="77589504"/>
+        <c:axId val="214010496"/>
+        <c:axId val="214581632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77587968"/>
+        <c:axId val="214010496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1362,13 +1679,13 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77589504"/>
+        <c:crossAx val="214581632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="30"/>
+        <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77589504"/>
+        <c:axId val="214581632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="3"/>
@@ -1398,7 +1715,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77587968"/>
+        <c:crossAx val="214010496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -1491,8 +1808,10 @@
             <c:v>Head</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:xVal>
@@ -1522,8 +1841,10 @@
             <c:v>Body</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -1752,11 +2073,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="79371648"/>
-        <c:axId val="79381632"/>
+        <c:axId val="214614784"/>
+        <c:axId val="214616320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="79371648"/>
+        <c:axId val="214614784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1776,13 +2097,13 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79381632"/>
+        <c:crossAx val="214616320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="30"/>
+        <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="79381632"/>
+        <c:axId val="214616320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2"/>
@@ -1817,7 +2138,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79371648"/>
+        <c:crossAx val="214614784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -1910,8 +2231,10 @@
             <c:v>Head</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:xVal>
@@ -2034,11 +2357,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="97058816"/>
-        <c:axId val="97060352"/>
+        <c:axId val="214545536"/>
+        <c:axId val="214547072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97058816"/>
+        <c:axId val="214545536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2058,16 +2381,16 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97060352"/>
+        <c:crossAx val="214547072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="30"/>
+        <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="97060352"/>
+        <c:axId val="214547072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="8"/>
+          <c:min val="9"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2099,7 +2422,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97058816"/>
+        <c:crossAx val="214545536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -2192,8 +2515,10 @@
             <c:v>Head</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:xVal>
@@ -2223,8 +2548,10 @@
             <c:v>Body</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -2453,11 +2780,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="97089792"/>
-        <c:axId val="97222656"/>
+        <c:axId val="215837696"/>
+        <c:axId val="215843584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97089792"/>
+        <c:axId val="215837696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2477,13 +2804,13 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97222656"/>
+        <c:crossAx val="215843584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="30"/>
+        <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="97222656"/>
+        <c:axId val="215843584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="4"/>
@@ -2518,7 +2845,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97089792"/>
+        <c:crossAx val="215837696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -2611,8 +2938,10 @@
             <c:v>Head</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:xVal>
@@ -2735,11 +3064,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="97245440"/>
-        <c:axId val="97247232"/>
+        <c:axId val="215976960"/>
+        <c:axId val="215978752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97245440"/>
+        <c:axId val="215976960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2759,16 +3088,16 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97247232"/>
+        <c:crossAx val="215978752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="30"/>
+        <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="97247232"/>
+        <c:axId val="215978752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="10"/>
+          <c:min val="11"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2800,7 +3129,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97245440"/>
+        <c:crossAx val="215976960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -2980,8 +3309,10 @@
             <c:v>Head min</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:xVal>
@@ -3011,8 +3342,10 @@
             <c:v>Head max</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -3054,8 +3387,10 @@
             <c:v>Body min</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -3099,8 +3434,10 @@
             <c:v>Body max</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -3143,11 +3480,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="98290688"/>
-        <c:axId val="99095680"/>
+        <c:axId val="216088576"/>
+        <c:axId val="216090496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="98290688"/>
+        <c:axId val="216088576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3157,6 +3494,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
         <c:txPr>
           <a:bodyPr rot="2700000"/>
           <a:lstStyle/>
@@ -3167,13 +3511,13 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99095680"/>
+        <c:crossAx val="216090496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="30"/>
+        <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99095680"/>
+        <c:axId val="216090496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3202,7 +3546,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98290688"/>
+        <c:crossAx val="216088576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3210,6 +3554,291 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="nb-NO"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>MTF</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 50% sharp UHR</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11404906290658777"/>
+          <c:y val="0.14030471800781"/>
+          <c:w val="0.63436816538584473"/>
+          <c:h val="0.70648357979642784"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Head</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Table!$A$12:$A$1000</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="989"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Table!$W$12:$W$1000</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="989"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>tol min head</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Table!$A$12,Table!$A$10)</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Table!$W$6,Table!$W$6)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>15.87</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.87</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>tol max head</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(Table!$A$12,Table!$A$10)</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Table!$W$7,Table!$W$7)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="216137088"/>
+        <c:axId val="216020096"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="216137088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="[$-414]mmm\.\ yy;@" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="2700000"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="216020096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="90"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="216020096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="23"/>
+          <c:min val="14"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>MTF</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> 50% (lp/mm)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="216137088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.77338321560576795"/>
+          <c:y val="8.0795083541386592E-2"/>
+          <c:w val="0.20707878067557164"/>
+          <c:h val="0.58806222392932594"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3477,6 +4106,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Diagram 11"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Diagram 12"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3772,28 +4465,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V43"/>
+  <sheetPr codeName="Ark1"/>
+  <dimension ref="A1:X43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="23" max="24" width="11.42578125" style="6"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -3806,8 +4503,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
@@ -3865,8 +4562,14 @@
       <c r="V6" s="3">
         <v>12.6</v>
       </c>
+      <c r="W6" s="3">
+        <v>15.87</v>
+      </c>
+      <c r="X6" s="3">
+        <v>20.47</v>
+      </c>
     </row>
-    <row r="7" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -3930,14 +4633,23 @@
       <c r="V7" s="3">
         <v>15.4</v>
       </c>
+      <c r="W7" s="3">
+        <v>22</v>
+      </c>
+      <c r="X7" s="3">
+        <v>25.01</v>
+      </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f>MAXA(A12:A1000)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
@@ -4004,8 +4716,14 @@
       <c r="V11" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="W11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="X11" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -4029,7 +4747,7 @@
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -4053,7 +4771,7 @@
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -4077,7 +4795,7 @@
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -4101,7 +4819,7 @@
       <c r="U15" s="6"/>
       <c r="V15" s="6"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -4774,75 +5492,90 @@
       <c r="V43" s="6"/>
     </row>
   </sheetData>
+  <sortState ref="A12:X25">
+    <sortCondition ref="A12:A25"/>
+  </sortState>
   <conditionalFormatting sqref="E12:H1000">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="notBetween">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="notBetween">
       <formula>-4</formula>
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:J1000">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12:K1000">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="notBetween">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="notBetween">
       <formula>$K$6</formula>
       <formula>$K$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L12:L1000">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="notBetween">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="notBetween">
       <formula>$L$6</formula>
       <formula>$L$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M12:N1000">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="notBetween">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="notBetween">
       <formula>$M$6</formula>
       <formula>$M$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O12:P1000">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="notBetween">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="notBetween">
       <formula>$O$6</formula>
       <formula>$O$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q12:Q1000">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="notBetween">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="notBetween">
       <formula>$Q$6</formula>
       <formula>$Q$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R12:R1000">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="notBetween">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="notBetween">
       <formula>$R$6</formula>
       <formula>$R$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S12:S1000">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="notBetween">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="notBetween">
       <formula>$S$6</formula>
       <formula>$S$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T12:T1000">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="notBetween">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="notBetween">
       <formula>$T$6</formula>
       <formula>$T$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U12:U1000">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="notBetween">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="notBetween">
       <formula>$U$6</formula>
       <formula>$U$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V12:V1000">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notBetween">
       <formula>$V$6</formula>
       <formula>$V$7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X12:X1000">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="notBetween">
+      <formula>$X$6</formula>
+      <formula>$X$7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W12:W1000">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="notBetween">
+      <formula>$W$6</formula>
+      <formula>$W$7</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4852,10 +5585,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Ark2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+      <selection activeCell="R33" sqref="R33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>